<commit_message>
[Docs] Damage doc updated.
</commit_message>
<xml_diff>
--- a/damages.xlsx
+++ b/damages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="16515" windowHeight="7995"/>
+    <workbookView minimized="1" xWindow="120" yWindow="45" windowWidth="16515" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Bucheron</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>HQ</t>
+  </si>
+  <si>
+    <t>Porteur</t>
+  </si>
+  <si>
+    <t>Constructeur</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,13 +678,16 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>14</v>
       </c>
-      <c r="G12" t="s">
-        <v>15</v>
+      <c r="H12" t="s">
+        <v>39</v>
       </c>
       <c r="K12" t="s">
         <v>14</v>
@@ -686,104 +698,65 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B13">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0.2</v>
+      </c>
+      <c r="G13">
         <v>10</v>
       </c>
-      <c r="E13">
-        <v>0.4</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13">
-        <v>20</v>
-      </c>
-      <c r="L13">
-        <v>20</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" t="s">
-        <v>35</v>
+      <c r="H13">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="J14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14">
-        <v>20</v>
-      </c>
-      <c r="L14">
-        <v>20</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>20</v>
+        <v>0.4</v>
       </c>
       <c r="G15">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K15">
         <v>20</v>
@@ -792,42 +765,48 @@
         <v>20</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N15" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="O15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>34</v>
@@ -835,100 +814,136 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>0.25</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="J17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17">
+        <v>20</v>
+      </c>
+      <c r="L17">
+        <v>20</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="J18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18">
         <v>10</v>
       </c>
-      <c r="D18">
+      <c r="L18">
         <v>10</v>
       </c>
-      <c r="E18">
-        <v>0.2</v>
-      </c>
-      <c r="F18">
-        <v>20</v>
-      </c>
-      <c r="G18">
-        <v>20</v>
-      </c>
-      <c r="J18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18">
-        <v>20</v>
-      </c>
-      <c r="L18">
-        <v>20</v>
-      </c>
       <c r="M18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" t="s">
-        <v>30</v>
-      </c>
-      <c r="O18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0.4</v>
+      </c>
+      <c r="G19">
         <v>8</v>
       </c>
-      <c r="B19">
-        <v>100</v>
-      </c>
-      <c r="C19">
-        <v>9</v>
-      </c>
-      <c r="J19" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19">
-        <v>20</v>
-      </c>
-      <c r="L19">
-        <v>20</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>31</v>
+      <c r="H19">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>0.2</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K20">
         <v>20</v>
@@ -936,43 +951,92 @@
       <c r="L20">
         <v>20</v>
       </c>
-      <c r="M20" t="s">
-        <v>32</v>
+      <c r="M20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>100</v>
       </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
       <c r="J21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K21">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L21">
-        <v>10</v>
-      </c>
-      <c r="M21" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22">
-        <v>50</v>
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22">
+        <v>20</v>
+      </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>10</v>
+      </c>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>500</v>
       </c>
     </row>

</xml_diff>